<commit_message>
Working in json to db
</commit_message>
<xml_diff>
--- a/RentData.xlsx
+++ b/RentData.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,348 +566,87 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>NIC</t>
+          <t>test</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>14000</t>
+          <t>test</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Tailor</t>
+          <t>test</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>test</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>14000</t>
+          <t>test</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>test</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Electric Bill is not paid</t>
+          <t>test</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Gas Bill is paid</t>
+          <t>test</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Electricity_Meter_Number</t>
+          <t>test</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Electricity_Account_Number</t>
+          <t>test</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Consumer_Number</t>
+          <t>test</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Electricity Meter Name</t>
+          <t>test</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Gas_Costumer_Number</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Gas_Meter_Number</t>
+          <t>test</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Advance_Amount</t>
+          <t>test</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>KK Moosa Plot No 72</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>987131123-4</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>12000</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Noor</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>76</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Electric Bill is paid</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Gas Bill is not paid</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>23084iadj08</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>jadh8</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>ajdhksa888</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Electricity Meter Name</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>89734jk3204-4</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>0ad</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Advance_Amount</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Compound</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>092348092348</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>12000</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Bareera</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Electric Bill is not paid</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Gas Bill is paid</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>87</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>13lkj</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>23lk4j</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>KHadi</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>203489</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>4000</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>KK Moosa Plot No 72</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>NIC</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1200</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Rentel_Name</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Due_Date</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Received_Rent</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Balance_Rent</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Electric_Bill</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Gas_Bill</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Electricity_Meter_Number</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Electricity_Account_Number</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Consumer_Number</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Electricity Meter Name</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Gas_Costumer_Number</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Gas_Meter_Number</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Advance_Amount</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>Show All Building</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>{'Date': '2024-07-29', 'Rent': '1200', 'Received_Rent': 'Received_Rent', 'Balance_Rent': 'Balance_Rent', 'Electric_Bill': 'Electric_Bill'}</t>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>[{'Date': '2024-07-31', 'Rent': 'test', 'Received_Rent': 'test', 'Balance_Rent': 'test'}]</t>
         </is>
       </c>
     </row>

</xml_diff>